<commit_message>
bo sung AI va tinh nang xoa
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fuzzefer/PycharmProjects/ChatBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2654ACD-ABC3-7A4D-AE42-D062278CB221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF22F373-3CF2-6D46-93ED-90C56B233CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="680" windowWidth="27620" windowHeight="17140" xr2:uid="{AB60E179-50C0-FB41-8279-970EBA839134}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,7 +468,7 @@
         <v>45994</v>
       </c>
       <c r="D2">
-        <v>500000</v>
+        <v>999999</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>

</xml_diff>